<commit_message>
Code integration and output
</commit_message>
<xml_diff>
--- a/Foward Backward LoadFlow Solver/data.xlsx
+++ b/Foward Backward LoadFlow Solver/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FYP\Code\UI\Foward Backward LoadFlow Software\Foward Backward LoadFlow Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FYP\Code\UI NEW\Foward Backward LoadFlow Solver\Foward Backward LoadFlow Solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746EC848-CB2C-4E35-93E5-1F56E4FD33D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308373F6-FD95-4FE8-A8C8-D3BDE89C6DCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="edges" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="voltages" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
     <sheet name="fbsweep" sheetId="5" r:id="rId5"/>
+    <sheet name="output" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Start Node</t>
   </si>
@@ -68,22 +69,13 @@
     <t>Round Factor</t>
   </si>
   <si>
-    <t>Nodes</t>
-  </si>
-  <si>
-    <t>Sweep 1</t>
-  </si>
-  <si>
-    <t>Sweep 2</t>
-  </si>
-  <si>
-    <t>Sweep 3</t>
-  </si>
-  <si>
-    <t>Sweep 4</t>
-  </si>
-  <si>
-    <t>Sweep 5</t>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>Polar Form</t>
+  </si>
+  <si>
+    <t>Cartesian Form</t>
   </si>
 </sst>
 </file>
@@ -439,7 +431,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +470,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +533,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B3"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,10 +563,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,27 +575,45 @@
     <col min="6" max="6" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889D7820-9578-4046-A737-4FD9DC38C17C}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code update and other menu items
</commit_message>
<xml_diff>
--- a/Foward Backward LoadFlow Solver/data.xlsx
+++ b/Foward Backward LoadFlow Solver/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FYP\Code\UI NEW\Foward Backward LoadFlow Solver\Foward Backward LoadFlow Solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308373F6-FD95-4FE8-A8C8-D3BDE89C6DCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7EBD2B-05F0-4075-BB19-9F64F2E85639}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="14010" windowHeight="7875" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="edges" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="voltages" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
     <sheet name="fbsweep" sheetId="5" r:id="rId5"/>
-    <sheet name="output" sheetId="6" r:id="rId6"/>
+    <sheet name="finaldata" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Start Node</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Cartesian Form</t>
+  </si>
+  <si>
+    <t>Upper Limit</t>
+  </si>
+  <si>
+    <t>Lower Limit</t>
   </si>
 </sst>
 </file>
@@ -502,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +560,16 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>